<commit_message>
major revisions to the data limitations, data comments columns of the data dictionaries
</commit_message>
<xml_diff>
--- a/data_final/consolidated/dictionaries/T_Dict.xlsx
+++ b/data_final/consolidated/dictionaries/T_Dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimer\github\opioid-policy-scan\data_final\consolidated\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2183B8-B1A0-4ED0-ACB3-99329B85FEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1AB10F-212C-4766-A93A-70190326B6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22957" yWindow="-14558" windowWidth="19366" windowHeight="21683" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tractsDataDictionary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="383">
   <si>
     <t>Theme</t>
   </si>
@@ -965,135 +965,6 @@
     <t/>
   </si>
   <si>
-    <t>9 na values</t>
-  </si>
-  <si>
-    <t>280 na values</t>
-  </si>
-  <si>
-    <t>368 na values</t>
-  </si>
-  <si>
-    <t>290 na values</t>
-  </si>
-  <si>
-    <t>285 na values</t>
-  </si>
-  <si>
-    <t>491 na values</t>
-  </si>
-  <si>
-    <t>520 na values</t>
-  </si>
-  <si>
-    <t>2 na values</t>
-  </si>
-  <si>
-    <t>379 na values</t>
-  </si>
-  <si>
-    <t>415 na values</t>
-  </si>
-  <si>
-    <t>367 na values</t>
-  </si>
-  <si>
-    <t>331 na values</t>
-  </si>
-  <si>
-    <t>20996 na values</t>
-  </si>
-  <si>
-    <t>21010 na values</t>
-  </si>
-  <si>
-    <t>525 na values</t>
-  </si>
-  <si>
-    <t>385 na values</t>
-  </si>
-  <si>
-    <t>442 na values</t>
-  </si>
-  <si>
-    <t>421 na values</t>
-  </si>
-  <si>
-    <t>440 na values</t>
-  </si>
-  <si>
-    <t>4 na values</t>
-  </si>
-  <si>
-    <t>47162 na values</t>
-  </si>
-  <si>
-    <t>789 na values</t>
-  </si>
-  <si>
-    <t>489 na values</t>
-  </si>
-  <si>
-    <t>492 na values</t>
-  </si>
-  <si>
-    <t>2400 na values</t>
-  </si>
-  <si>
-    <t>762 na values</t>
-  </si>
-  <si>
-    <t>3643 na values</t>
-  </si>
-  <si>
-    <t>29763 na values</t>
-  </si>
-  <si>
-    <t>11371 na values</t>
-  </si>
-  <si>
-    <t>710 na values</t>
-  </si>
-  <si>
-    <t>8550 na values</t>
-  </si>
-  <si>
-    <t>2662 na values</t>
-  </si>
-  <si>
-    <t>38 na values</t>
-  </si>
-  <si>
-    <t>8 na values</t>
-  </si>
-  <si>
-    <t>17 na values</t>
-  </si>
-  <si>
-    <t>23 na values</t>
-  </si>
-  <si>
-    <t>20 na values</t>
-  </si>
-  <si>
-    <t>1774 na values</t>
-  </si>
-  <si>
-    <t>227 na values</t>
-  </si>
-  <si>
-    <t>219 na values</t>
-  </si>
-  <si>
-    <t>787 na values</t>
-  </si>
-  <si>
-    <t>466 na values</t>
-  </si>
-  <si>
-    <t>494 na values</t>
-  </si>
-  <si>
     <t>TotVetPop</t>
   </si>
   <si>
@@ -1272,6 +1143,46 @@
   </si>
   <si>
     <t>Longitudinal</t>
+  </si>
+  <si>
+    <t>Some tracts are not assigned with any typologies because data are missing for factor analysis.</t>
+  </si>
+  <si>
+    <t>This is the taken by a team of individuals in a continuum of care in one day. It is difficult to measure homelessness at a local and Federal level as the population is relatively mobile, homelessness can be cyclical and there are visibility issues for the homeless community, so the annual point in time count was used as a proxy for homelessness in this dataset. Data was geocoded then spatially joined at the tract, ZCTA, state and county level to see where continuums of care are located and the availibility of temporary housing solutions.</t>
+  </si>
+  <si>
+    <t>Please note this dataset uses industry as a classifier and does not include any information about the specific occupation in that industry. This could lead to an overestimation of High Risk to Injury workers category.</t>
+  </si>
+  <si>
+    <t>The data reflects 2007-2008 estimates. Note again, via NSP2 Data and Methodology: The estimated rate of foreclosure problems do not reflect "real" numbers of foreclosures but rather reflect neighborhood characteristics that are estimated to have a high level of risk for foreclosure.</t>
+  </si>
+  <si>
+    <t>For more recent county, state, and metro area data on mortgage delinquencies, see Mortgage Performance Trends data from the U.S. Consumer Financial Protection Bureau.</t>
+  </si>
+  <si>
+    <t>Alcohol outlet density is one approximation for accessibility or demand, though a limited one for describing or understanding the complex relationship between alcohol consumption and the surrounding area or communithy.
+The category of 'alcohol outlets' included in this dataset does not include supermarkets and/or drug stores that may carry beer, wine, or liquor. The laws governing these sales varies from state to state, permitting alcohol sales in different kind of sales outlets. Outlets that are permitted to make these sales may not always fall under the same NAICS code for Beer, Wine, and Liquor Stores.</t>
+  </si>
+  <si>
+    <t>Despite removing identified influences of cloud interferences, there may still be clouds or other atmospheric conditions that alter pixel values used in calculations. See the original source for greater documentation of these effects. Furthermore, summarizing NDVI to the census tract simplifies inter-census tract variability.</t>
+  </si>
+  <si>
+    <t>Access metrics are calculated for continental U.S., and does not include Hawaii, Alaska, or U.S. territories.</t>
+  </si>
+  <si>
+    <t>All nearest distance calculations are in miles. All nearest travel time calculations are in minutes.</t>
+  </si>
+  <si>
+    <t>*Euclidean distance or straight-line distance is a simple approximation of distance or travel time from an origin centroid to the nearest health center. It is not a precise calculation of real travel times or distances.</t>
+  </si>
+  <si>
+    <t>This dataset includes all US states, Washington D.C., and Puerto Rico. It does not include the territories Guam, Northern Mariana Islands, American Samoa, Palau. Zip code and tract centroids are not population-weighted.</t>
+  </si>
+  <si>
+    <t>Does not include U.S. territories Puerto Rico, Guam, Northern Mariana Islands, American Samoa, Virgin Islands, or Washington, D.C.</t>
+  </si>
+  <si>
+    <t>Please note that the SVI dataset at the ZIP code level is an estimate based on crosswalking the original CDC SVI Census tract measures to ZIP codes; some gaps in this data are to be expected. The ZIP code data does not include Puerto Rico or other US territories.</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1600,6 +1511,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1761,7 +1678,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1770,6 +1687,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2129,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2140,8 +2063,9 @@
     <col min="6" max="6" width="4.8125" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="3"/>
-    <col min="9" max="10" width="11" style="1"/>
-    <col min="11" max="11" width="52.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1"/>
+    <col min="10" max="10" width="187.8125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.75" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="168.6875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.25" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5" style="1" bestFit="1" customWidth="1"/>
@@ -2168,10 +2092,10 @@
         <v>2010</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>411</v>
+        <v>368</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>412</v>
+        <v>369</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>257</v>
@@ -2189,7 +2113,7 @@
         <v>4</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>355</v>
+        <v>312</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>5</v>
@@ -2208,6 +2132,25 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H2" s="7"/>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2215,10 +2158,10 @@
         <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>388</v>
+        <v>345</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>11</v>
@@ -2234,6 +2177,25 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H3" s="7"/>
       <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2241,10 +2203,10 @@
         <v>17</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>388</v>
+        <v>345</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>11</v>
@@ -2260,6 +2222,17 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H4" s="7"/>
       <c r="I4" s="1" t="s">
         <v>258</v>
       </c>
@@ -2279,13 +2252,32 @@
         <v>36526</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>406</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H5" s="7"/>
       <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2293,10 +2285,10 @@
         <v>15</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>388</v>
+        <v>345</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>11</v>
@@ -2312,6 +2304,25 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B6" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H6" s="7"/>
       <c r="I6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2319,10 +2330,10 @@
         <v>13</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>388</v>
+        <v>345</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>11</v>
@@ -2360,19 +2371,19 @@
         <v>302</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>410</v>
+        <v>367</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>308</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>277</v>
@@ -2384,7 +2395,7 @@
         <v>309</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.5">
@@ -2398,19 +2409,19 @@
         <v>302</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>353</v>
+        <v>310</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>354</v>
+        <v>311</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>393</v>
+        <v>350</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>395</v>
+        <v>352</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>359</v>
+        <v>316</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>277</v>
@@ -2439,7 +2450,7 @@
         <v>24</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>360</v>
+        <v>317</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>277</v>
@@ -2480,13 +2491,13 @@
         <v>256</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>400</v>
+        <v>357</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>409</v>
+        <v>366</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>277</v>
@@ -2498,7 +2509,7 @@
         <v>309</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>401</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.5">
@@ -2521,16 +2532,13 @@
         <v>24</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>277</v>
       </c>
       <c r="O11" s="1">
         <v>5556</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.5">
@@ -2565,13 +2573,13 @@
         <v>29</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>278</v>
@@ -2579,11 +2587,8 @@
       <c r="O12" s="1">
         <v>80.290000000000006</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.5">
@@ -2618,13 +2623,13 @@
         <v>31</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>278</v>
@@ -2632,11 +2637,8 @@
       <c r="O13" s="1">
         <v>13.78</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.5">
@@ -2671,13 +2673,13 @@
         <v>33</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>278</v>
@@ -2685,11 +2687,8 @@
       <c r="O14" s="1">
         <v>0</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q14" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.5">
@@ -2724,13 +2723,13 @@
         <v>35</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>278</v>
@@ -2738,11 +2737,8 @@
       <c r="O15" s="1">
         <v>0.38</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q15" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.5">
@@ -2771,19 +2767,19 @@
         <v>302</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>385</v>
+        <v>342</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>278</v>
@@ -2791,11 +2787,8 @@
       <c r="O16" s="1">
         <v>0</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q16" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.5">
@@ -2830,13 +2823,13 @@
         <v>38</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>278</v>
@@ -2844,11 +2837,8 @@
       <c r="O17" s="1">
         <v>5.55</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q17" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.5">
@@ -2883,13 +2873,13 @@
         <v>40</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>278</v>
@@ -2897,11 +2887,8 @@
       <c r="O18" s="1">
         <v>8.18</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q18" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.5">
@@ -2932,9 +2919,6 @@
       <c r="O19" s="1">
         <v>0.23</v>
       </c>
-      <c r="P19" s="1" t="s">
-        <v>311</v>
-      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
@@ -2968,13 +2952,13 @@
         <v>43</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>278</v>
@@ -2982,11 +2966,8 @@
       <c r="O20" s="1">
         <v>14.63</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q20" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.5">
@@ -3018,13 +2999,13 @@
         <v>45</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>278</v>
@@ -3032,11 +3013,8 @@
       <c r="O21" s="1">
         <v>66.83</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q21" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.5">
@@ -3068,13 +3046,13 @@
         <v>47</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>278</v>
@@ -3082,11 +3060,8 @@
       <c r="O22" s="1">
         <v>11.45</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="Q22" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.5">
@@ -3118,13 +3093,13 @@
         <v>49</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>277</v>
@@ -3132,11 +3107,8 @@
       <c r="O23" s="1">
         <v>607</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q23" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.5">
@@ -3168,13 +3140,13 @@
         <v>51</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>277</v>
@@ -3182,11 +3154,8 @@
       <c r="O24" s="1">
         <v>1070</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q24" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.5">
@@ -3218,13 +3187,13 @@
         <v>53</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>277</v>
@@ -3232,11 +3201,8 @@
       <c r="O25" s="1">
         <v>722</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q25" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.5">
@@ -3268,13 +3234,13 @@
         <v>55</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>277</v>
@@ -3282,11 +3248,8 @@
       <c r="O26" s="1">
         <v>704</v>
       </c>
-      <c r="P26" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q26" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.5">
@@ -3318,13 +3281,13 @@
         <v>57</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>277</v>
@@ -3332,11 +3295,8 @@
       <c r="O27" s="1">
         <v>4835</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q27" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.5">
@@ -3362,22 +3322,19 @@
         <v>59</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>277</v>
       </c>
       <c r="O28" s="1">
         <v>495</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.5">
@@ -3403,22 +3360,19 @@
         <v>61</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>277</v>
       </c>
       <c r="O29" s="1">
         <v>531</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.5">
@@ -3429,22 +3383,22 @@
         <v>302</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>380</v>
+        <v>337</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>381</v>
+        <v>338</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>382</v>
+        <v>339</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>383</v>
+        <v>340</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>277</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>404</v>
+        <v>361</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.5">
@@ -3476,13 +3430,13 @@
         <v>63</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>277</v>
@@ -3490,11 +3444,8 @@
       <c r="O31" s="1">
         <v>718</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q31" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.5">
@@ -3526,13 +3477,13 @@
         <v>65</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>277</v>
@@ -3540,11 +3491,8 @@
       <c r="O32" s="1">
         <v>372</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q32" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.5">
@@ -3576,13 +3524,13 @@
         <v>67</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>277</v>
@@ -3590,11 +3538,8 @@
       <c r="O33" s="1">
         <v>1116</v>
       </c>
-      <c r="P33" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q33" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.5">
@@ -3617,19 +3562,16 @@
         <v>19</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>397</v>
+        <v>354</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>277</v>
       </c>
       <c r="O34" s="1">
         <v>7468</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.5">
@@ -3664,13 +3606,13 @@
         <v>71</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>277</v>
@@ -3678,11 +3620,8 @@
       <c r="O35" s="1">
         <v>6352</v>
       </c>
-      <c r="P35" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="Q35" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.5">
@@ -3708,13 +3647,13 @@
         <v>73</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>390</v>
+        <v>347</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>394</v>
+        <v>351</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>278</v>
@@ -3722,11 +3661,8 @@
       <c r="O36" s="1">
         <v>8.9</v>
       </c>
-      <c r="P36" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="Q36" s="1" t="s">
-        <v>405</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.5">
@@ -3755,19 +3691,19 @@
         <v>302</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>386</v>
+        <v>343</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>74</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>394</v>
+        <v>351</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>278</v>
@@ -3775,11 +3711,8 @@
       <c r="O37" s="1">
         <v>3.78</v>
       </c>
-      <c r="P37" s="1" t="s">
-        <v>313</v>
-      </c>
       <c r="Q37" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.5">
@@ -3802,22 +3735,19 @@
         <v>76</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>391</v>
+        <v>348</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>398</v>
+        <v>355</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>359</v>
+        <v>316</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O38" s="1">
         <v>15.7</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.5">
@@ -3840,22 +3770,19 @@
         <v>78</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>392</v>
+        <v>349</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>398</v>
+        <v>355</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>360</v>
+        <v>317</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O39" s="1">
         <v>4.26</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.5">
@@ -3878,22 +3805,19 @@
         <v>80</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>392</v>
+        <v>349</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>398</v>
+        <v>355</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>360</v>
+        <v>317</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O40" s="1">
         <v>18.39</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.5">
@@ -3916,7 +3840,7 @@
         <v>84</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>361</v>
+        <v>318</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>277</v>
@@ -3925,7 +3849,7 @@
         <v>0</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.5">
@@ -3948,7 +3872,7 @@
         <v>84</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>361</v>
+        <v>318</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>277</v>
@@ -3957,7 +3881,7 @@
         <v>0</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.5">
@@ -3980,7 +3904,7 @@
         <v>84</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>361</v>
+        <v>318</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>277</v>
@@ -3989,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.5">
@@ -4024,13 +3948,13 @@
         <v>103</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>390</v>
+        <v>347</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>394</v>
+        <v>351</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>364</v>
+        <v>321</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>278</v>
@@ -4038,11 +3962,8 @@
       <c r="O44" s="1">
         <v>5.6</v>
       </c>
-      <c r="P44" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="Q44" s="1" t="s">
-        <v>401</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.5">
@@ -4077,13 +3998,13 @@
         <v>105</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>390</v>
+        <v>347</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>394</v>
+        <v>351</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>364</v>
+        <v>321</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>278</v>
@@ -4091,11 +4012,8 @@
       <c r="O45" s="1">
         <v>14.2</v>
       </c>
-      <c r="P45" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="Q45" s="1" t="s">
-        <v>401</v>
+        <v>358</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.5">
@@ -4115,22 +4033,19 @@
         <v>300</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>384</v>
+        <v>341</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>393</v>
+        <v>350</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>399</v>
+        <v>356</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O46" s="1">
         <v>31504</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.5">
@@ -4156,13 +4071,13 @@
         <v>301</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>390</v>
+        <v>347</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>394</v>
+        <v>351</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>364</v>
+        <v>321</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>278</v>
@@ -4170,11 +4085,8 @@
       <c r="O47" s="1">
         <v>29969</v>
       </c>
-      <c r="P47" s="1" t="s">
-        <v>321</v>
-      </c>
       <c r="Q47" s="1" t="s">
-        <v>402</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.5">
@@ -4197,7 +4109,7 @@
         <v>109</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>365</v>
+        <v>322</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>278</v>
@@ -4206,7 +4118,10 @@
         <v>9.1</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>322</v>
+        <v>373</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.5">
@@ -4229,7 +4144,7 @@
         <v>109</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>365</v>
+        <v>322</v>
       </c>
       <c r="N49" s="1" t="s">
         <v>277</v>
@@ -4238,7 +4153,10 @@
         <v>128</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>323</v>
+        <v>373</v>
+      </c>
+      <c r="Q49" s="6" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.5">
@@ -4269,9 +4187,6 @@
       <c r="O50" s="1">
         <v>0.38</v>
       </c>
-      <c r="P50" s="1" t="s">
-        <v>324</v>
-      </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
@@ -4293,7 +4208,7 @@
         <v>24</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>278</v>
@@ -4301,8 +4216,8 @@
       <c r="O51" s="1">
         <v>8.0299999999999994</v>
       </c>
-      <c r="P51" s="1" t="s">
-        <v>325</v>
+      <c r="P51" s="6" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.5">
@@ -4328,7 +4243,7 @@
         <v>24</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>278</v>
@@ -4336,8 +4251,8 @@
       <c r="O52" s="1">
         <v>16.18</v>
       </c>
-      <c r="P52" s="1" t="s">
-        <v>325</v>
+      <c r="P52" s="6" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.5">
@@ -4360,7 +4275,7 @@
         <v>24</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>278</v>
@@ -4368,8 +4283,8 @@
       <c r="O53" s="1">
         <v>14.7</v>
       </c>
-      <c r="P53" s="1" t="s">
-        <v>325</v>
+      <c r="P53" s="6" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.5">
@@ -4392,7 +4307,7 @@
         <v>24</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>278</v>
@@ -4400,8 +4315,8 @@
       <c r="O54" s="1">
         <v>15.39</v>
       </c>
-      <c r="P54" s="1" t="s">
-        <v>325</v>
+      <c r="P54" s="6" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.5">
@@ -4424,16 +4339,13 @@
         <v>24</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>363</v>
+        <v>320</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>277</v>
       </c>
       <c r="O55" s="1">
         <v>2092</v>
-      </c>
-      <c r="P55" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.5">
@@ -4459,16 +4371,13 @@
         <v>24</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>363</v>
+        <v>320</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O56" s="1">
         <v>37.65</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.5">
@@ -4494,16 +4403,13 @@
         <v>117</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>366</v>
+        <v>323</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O57" s="1">
         <v>6.64</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.5">
@@ -4538,13 +4444,13 @@
         <v>119</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>407</v>
+        <v>364</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>408</v>
+        <v>365</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>278</v>
@@ -4552,11 +4458,8 @@
       <c r="O58" s="1">
         <v>11.72</v>
       </c>
-      <c r="P58" s="1" t="s">
-        <v>327</v>
-      </c>
       <c r="Q58" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.5">
@@ -4579,16 +4482,13 @@
         <v>20</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O59" s="1">
         <v>0.68</v>
-      </c>
-      <c r="P59" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.5">
@@ -4611,16 +4511,13 @@
         <v>20</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O60" s="1">
         <v>8.66</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.5">
@@ -4643,16 +4540,13 @@
         <v>20</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="N61" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O61" s="1">
         <v>19.899999999999999</v>
-      </c>
-      <c r="P61" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.5">
@@ -4675,16 +4569,13 @@
         <v>20</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>278</v>
       </c>
       <c r="O62" s="1">
         <v>673.09</v>
-      </c>
-      <c r="P62" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.5">
@@ -4707,16 +4598,13 @@
         <v>131</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>368</v>
+        <v>325</v>
       </c>
       <c r="N63" s="1" t="s">
         <v>244</v>
       </c>
       <c r="O63" s="1">
         <v>1</v>
-      </c>
-      <c r="P63" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.5">
@@ -4739,7 +4627,7 @@
         <v>131</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>368</v>
+        <v>325</v>
       </c>
       <c r="N64" s="1" t="s">
         <v>244</v>
@@ -4747,11 +4635,8 @@
       <c r="O64" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P64" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.5">
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
@@ -4774,7 +4659,7 @@
         <v>131</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>368</v>
+        <v>325</v>
       </c>
       <c r="N65" s="1" t="s">
         <v>280</v>
@@ -4782,11 +4667,8 @@
       <c r="O65" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="P65" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.5">
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
         <v>8</v>
       </c>
@@ -4806,7 +4688,7 @@
         <v>139</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
       <c r="N66" s="1" t="s">
         <v>278</v>
@@ -4815,10 +4697,10 @@
         <v>6.73</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.5">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A67" s="1" t="s">
         <v>113</v>
       </c>
@@ -4838,7 +4720,7 @@
         <v>139</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
       <c r="N67" s="1" t="s">
         <v>277</v>
@@ -4847,10 +4729,10 @@
         <v>1</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.5">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A68" s="1" t="s">
         <v>113</v>
       </c>
@@ -4870,7 +4752,7 @@
         <v>139</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
       <c r="N68" s="1" t="s">
         <v>278</v>
@@ -4879,10 +4761,10 @@
         <v>0.15</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.5">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A69" s="1" t="s">
         <v>113</v>
       </c>
@@ -4902,7 +4784,7 @@
         <v>139</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>278</v>
@@ -4911,10 +4793,10 @@
         <v>0</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.5">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
         <v>113</v>
       </c>
@@ -4937,7 +4819,7 @@
         <v>148</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>278</v>
@@ -4945,11 +4827,11 @@
       <c r="O70" s="1">
         <v>0.15</v>
       </c>
-      <c r="P70" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P70" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>113</v>
       </c>
@@ -4969,7 +4851,7 @@
         <v>152</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N71" s="1" t="s">
         <v>278</v>
@@ -4977,11 +4859,14 @@
       <c r="O71" s="1">
         <v>0.81</v>
       </c>
-      <c r="P71" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P71" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q71" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -5001,7 +4886,7 @@
         <v>152</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N72" s="1" t="s">
         <v>278</v>
@@ -5009,11 +4894,14 @@
       <c r="O72" s="1">
         <v>0.81</v>
       </c>
-      <c r="P72" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P72" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q72" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
         <v>113</v>
       </c>
@@ -5036,7 +4924,7 @@
         <v>152</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N73" s="1" t="s">
         <v>278</v>
@@ -5044,11 +4932,14 @@
       <c r="O73" s="1">
         <v>0</v>
       </c>
-      <c r="P73" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P73" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q73" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A74" s="1" t="s">
         <v>113</v>
       </c>
@@ -5068,7 +4959,7 @@
         <v>152</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N74" s="1" t="s">
         <v>277</v>
@@ -5076,11 +4967,14 @@
       <c r="O74" s="1">
         <v>21</v>
       </c>
-      <c r="P74" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P74" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q74" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A75" s="1" t="s">
         <v>113</v>
       </c>
@@ -5100,7 +4994,7 @@
         <v>152</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N75" s="1" t="s">
         <v>278</v>
@@ -5108,11 +5002,14 @@
       <c r="O75" s="1">
         <v>13.22</v>
       </c>
-      <c r="P75" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P75" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q75" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A76" s="1" t="s">
         <v>113</v>
       </c>
@@ -5135,7 +5032,7 @@
         <v>152</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N76" s="1" t="s">
         <v>278</v>
@@ -5143,11 +5040,14 @@
       <c r="O76" s="1">
         <v>27.39</v>
       </c>
-      <c r="P76" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P76" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q76" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A77" s="1" t="s">
         <v>113</v>
       </c>
@@ -5167,7 +5067,7 @@
         <v>152</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N77" s="1" t="s">
         <v>277</v>
@@ -5175,11 +5075,14 @@
       <c r="O77" s="1">
         <v>1</v>
       </c>
-      <c r="P77" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P77" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q77" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
         <v>113</v>
       </c>
@@ -5199,7 +5102,7 @@
         <v>152</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N78" s="1" t="s">
         <v>278</v>
@@ -5207,11 +5110,14 @@
       <c r="O78" s="1">
         <v>18.04</v>
       </c>
-      <c r="P78" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P78" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q78" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>113</v>
       </c>
@@ -5234,7 +5140,7 @@
         <v>152</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>278</v>
@@ -5242,11 +5148,14 @@
       <c r="O79" s="1">
         <v>35.340000000000003</v>
       </c>
-      <c r="P79" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P79" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q79" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>113</v>
       </c>
@@ -5266,7 +5175,7 @@
         <v>152</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N80" s="1" t="s">
         <v>277</v>
@@ -5274,11 +5183,14 @@
       <c r="O80" s="1">
         <v>0</v>
       </c>
-      <c r="P80" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="P80" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q80" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A81" s="1" t="s">
         <v>113</v>
       </c>
@@ -5301,7 +5213,7 @@
         <v>152</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N81" s="1" t="s">
         <v>278</v>
@@ -5309,11 +5221,14 @@
       <c r="O81" s="1">
         <v>0</v>
       </c>
-      <c r="P81" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P81" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q81" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A82" s="1" t="s">
         <v>113</v>
       </c>
@@ -5333,7 +5248,7 @@
         <v>152</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N82" s="1" t="s">
         <v>277</v>
@@ -5341,11 +5256,14 @@
       <c r="O82" s="1">
         <v>2</v>
       </c>
-      <c r="P82" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P82" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q82" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A83" s="1" t="s">
         <v>113</v>
       </c>
@@ -5365,7 +5283,7 @@
         <v>152</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N83" s="1" t="s">
         <v>277</v>
@@ -5373,11 +5291,14 @@
       <c r="O83" s="1">
         <v>2</v>
       </c>
-      <c r="P83" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P83" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q83" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A84" s="1" t="s">
         <v>113</v>
       </c>
@@ -5400,7 +5321,7 @@
         <v>152</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N84" s="1" t="s">
         <v>278</v>
@@ -5408,11 +5329,14 @@
       <c r="O84" s="1">
         <v>1744.66</v>
       </c>
-      <c r="P84" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P84" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q84" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A85" s="1" t="s">
         <v>113</v>
       </c>
@@ -5432,7 +5356,7 @@
         <v>152</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N85" s="1" t="s">
         <v>277</v>
@@ -5440,11 +5364,14 @@
       <c r="O85" s="1">
         <v>0</v>
       </c>
-      <c r="P85" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P85" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q85" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
         <v>113</v>
       </c>
@@ -5464,7 +5391,7 @@
         <v>152</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N86" s="1" t="s">
         <v>277</v>
@@ -5472,11 +5399,14 @@
       <c r="O86" s="1">
         <v>0</v>
       </c>
-      <c r="P86" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P86" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q86" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
         <v>113</v>
       </c>
@@ -5499,7 +5429,7 @@
         <v>152</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N87" s="1" t="s">
         <v>278</v>
@@ -5507,11 +5437,14 @@
       <c r="O87" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="P87" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P87" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q87" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A88" s="1" t="s">
         <v>113</v>
       </c>
@@ -5531,7 +5464,7 @@
         <v>152</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N88" s="1" t="s">
         <v>277</v>
@@ -5539,11 +5472,14 @@
       <c r="O88" s="1">
         <v>0</v>
       </c>
-      <c r="P88" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P88" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q88" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
         <v>113</v>
       </c>
@@ -5563,7 +5499,7 @@
         <v>152</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N89" s="1" t="s">
         <v>277</v>
@@ -5571,11 +5507,14 @@
       <c r="O89" s="1">
         <v>0</v>
       </c>
-      <c r="P89" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P89" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q89" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A90" s="1" t="s">
         <v>113</v>
       </c>
@@ -5598,7 +5537,7 @@
         <v>152</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N90" s="1" t="s">
         <v>278</v>
@@ -5606,11 +5545,14 @@
       <c r="O90" s="1">
         <v>0</v>
       </c>
-      <c r="P90" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P90" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q90" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A91" s="1" t="s">
         <v>113</v>
       </c>
@@ -5630,7 +5572,7 @@
         <v>152</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N91" s="1" t="s">
         <v>277</v>
@@ -5638,11 +5580,14 @@
       <c r="O91" s="1">
         <v>4</v>
       </c>
-      <c r="P91" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P91" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q91" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A92" s="1" t="s">
         <v>113</v>
       </c>
@@ -5662,7 +5607,7 @@
         <v>152</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N92" s="1" t="s">
         <v>277</v>
@@ -5670,11 +5615,14 @@
       <c r="O92" s="1">
         <v>3</v>
       </c>
-      <c r="P92" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P92" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q92" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A93" s="1" t="s">
         <v>113</v>
       </c>
@@ -5697,7 +5645,7 @@
         <v>152</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N93" s="1" t="s">
         <v>278</v>
@@ -5705,11 +5653,14 @@
       <c r="O93" s="1">
         <v>148.18</v>
       </c>
-      <c r="P93" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P93" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q93" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
         <v>113</v>
       </c>
@@ -5729,7 +5680,7 @@
         <v>152</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N94" s="1" t="s">
         <v>277</v>
@@ -5737,11 +5688,14 @@
       <c r="O94" s="1">
         <v>0</v>
       </c>
-      <c r="P94" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P94" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q94" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
         <v>113</v>
       </c>
@@ -5761,7 +5715,7 @@
         <v>152</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N95" s="1" t="s">
         <v>277</v>
@@ -5769,11 +5723,14 @@
       <c r="O95" s="1">
         <v>0</v>
       </c>
-      <c r="P95" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P95" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q95" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A96" s="1" t="s">
         <v>113</v>
       </c>
@@ -5796,7 +5753,7 @@
         <v>152</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N96" s="1" t="s">
         <v>278</v>
@@ -5804,11 +5761,14 @@
       <c r="O96" s="1">
         <v>165.18</v>
       </c>
-      <c r="P96" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P96" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q96" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A97" s="1" t="s">
         <v>113</v>
       </c>
@@ -5828,7 +5788,7 @@
         <v>152</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N97" s="1" t="s">
         <v>277</v>
@@ -5836,11 +5796,14 @@
       <c r="O97" s="1">
         <v>0</v>
       </c>
-      <c r="P97" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P97" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q97" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
         <v>113</v>
       </c>
@@ -5860,7 +5823,7 @@
         <v>152</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="N98" s="1" t="s">
         <v>277</v>
@@ -5868,11 +5831,14 @@
       <c r="O98" s="1">
         <v>0</v>
       </c>
-      <c r="P98" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P98" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q98" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A99" s="1" t="s">
         <v>113</v>
       </c>
@@ -5892,7 +5858,7 @@
         <v>206</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>372</v>
+        <v>329</v>
       </c>
       <c r="N99" s="1" t="s">
         <v>278</v>
@@ -5900,11 +5866,14 @@
       <c r="O99" s="1">
         <v>10.23</v>
       </c>
-      <c r="P99" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P99" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q99" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A100" s="1" t="s">
         <v>113</v>
       </c>
@@ -5927,7 +5896,7 @@
         <v>206</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>372</v>
+        <v>329</v>
       </c>
       <c r="N100" s="1" t="s">
         <v>278</v>
@@ -5935,11 +5904,14 @@
       <c r="O100" s="1">
         <v>19.16</v>
       </c>
-      <c r="P100" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P100" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q100" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A101" s="1" t="s">
         <v>113</v>
       </c>
@@ -5959,7 +5931,7 @@
         <v>206</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>372</v>
+        <v>329</v>
       </c>
       <c r="N101" s="1" t="s">
         <v>277</v>
@@ -5967,11 +5939,14 @@
       <c r="O101" s="1">
         <v>17</v>
       </c>
-      <c r="P101" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P101" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q101" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
         <v>113</v>
       </c>
@@ -5991,7 +5966,7 @@
         <v>211</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>373</v>
+        <v>330</v>
       </c>
       <c r="N102" s="1" t="s">
         <v>278</v>
@@ -5999,11 +5974,14 @@
       <c r="O102" s="1">
         <v>0.31</v>
       </c>
-      <c r="P102" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P102" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q102" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
         <v>113</v>
       </c>
@@ -6026,7 +6004,7 @@
         <v>211</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>373</v>
+        <v>330</v>
       </c>
       <c r="N103" s="1" t="s">
         <v>278</v>
@@ -6034,11 +6012,14 @@
       <c r="O103" s="1">
         <v>0</v>
       </c>
-      <c r="P103" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P103" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q103" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
         <v>113</v>
       </c>
@@ -6058,7 +6039,7 @@
         <v>211</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>373</v>
+        <v>330</v>
       </c>
       <c r="N104" s="1" t="s">
         <v>277</v>
@@ -6066,11 +6047,14 @@
       <c r="O104" s="1">
         <v>6</v>
       </c>
-      <c r="P104" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P104" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q104" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A105" s="1" t="s">
         <v>113</v>
       </c>
@@ -6090,7 +6074,7 @@
         <v>215</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>374</v>
+        <v>331</v>
       </c>
       <c r="N105" s="1" t="s">
         <v>278</v>
@@ -6098,11 +6082,14 @@
       <c r="O105" s="1">
         <v>0.84</v>
       </c>
-      <c r="P105" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P105" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q105" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
         <v>113</v>
       </c>
@@ -6125,7 +6112,7 @@
         <v>215</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>374</v>
+        <v>331</v>
       </c>
       <c r="N106" s="1" t="s">
         <v>278</v>
@@ -6133,11 +6120,14 @@
       <c r="O106" s="1">
         <v>0</v>
       </c>
-      <c r="P106" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P106" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q106" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
         <v>113</v>
       </c>
@@ -6157,7 +6147,7 @@
         <v>215</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>374</v>
+        <v>331</v>
       </c>
       <c r="N107" s="1" t="s">
         <v>277</v>
@@ -6165,11 +6155,14 @@
       <c r="O107" s="1">
         <v>58</v>
       </c>
-      <c r="P107" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P107" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q107" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A108" s="1" t="s">
         <v>113</v>
       </c>
@@ -6189,7 +6182,7 @@
         <v>221</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>375</v>
+        <v>332</v>
       </c>
       <c r="N108" s="1" t="s">
         <v>278</v>
@@ -6197,11 +6190,14 @@
       <c r="O108" s="1">
         <v>0.2</v>
       </c>
-      <c r="P108" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P108" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q108" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
@@ -6224,7 +6220,7 @@
         <v>221</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>375</v>
+        <v>332</v>
       </c>
       <c r="N109" s="1" t="s">
         <v>278</v>
@@ -6232,11 +6228,14 @@
       <c r="O109" s="1">
         <v>0</v>
       </c>
-      <c r="P109" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P109" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q109" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
         <v>113</v>
       </c>
@@ -6256,7 +6255,7 @@
         <v>221</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>375</v>
+        <v>332</v>
       </c>
       <c r="N110" s="1" t="s">
         <v>277</v>
@@ -6264,11 +6263,14 @@
       <c r="O110" s="1">
         <v>3</v>
       </c>
-      <c r="P110" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P110" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q110" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
         <v>113</v>
       </c>
@@ -6288,7 +6290,7 @@
         <v>221</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>376</v>
+        <v>333</v>
       </c>
       <c r="N111" s="1" t="s">
         <v>278</v>
@@ -6296,11 +6298,14 @@
       <c r="O111" s="1">
         <v>4.99</v>
       </c>
-      <c r="P111" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P111" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q111" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A112" s="1" t="s">
         <v>113</v>
       </c>
@@ -6323,7 +6328,7 @@
         <v>221</v>
       </c>
       <c r="M112" s="1" t="s">
-        <v>376</v>
+        <v>333</v>
       </c>
       <c r="N112" s="1" t="s">
         <v>278</v>
@@ -6331,11 +6336,14 @@
       <c r="O112" s="1">
         <v>17.760000000000002</v>
       </c>
-      <c r="P112" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P112" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q112" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A113" s="1" t="s">
         <v>113</v>
       </c>
@@ -6355,7 +6363,7 @@
         <v>221</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>376</v>
+        <v>333</v>
       </c>
       <c r="N113" s="1" t="s">
         <v>277</v>
@@ -6363,11 +6371,14 @@
       <c r="O113" s="1">
         <v>4</v>
       </c>
-      <c r="P113" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P113" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q113" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
@@ -6387,7 +6398,7 @@
         <v>230</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>377</v>
+        <v>334</v>
       </c>
       <c r="N114" s="1" t="s">
         <v>278</v>
@@ -6395,11 +6406,14 @@
       <c r="O114" s="1">
         <v>13.12</v>
       </c>
-      <c r="P114" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P114" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q114" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
@@ -6422,7 +6436,7 @@
         <v>230</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>377</v>
+        <v>334</v>
       </c>
       <c r="N115" s="1" t="s">
         <v>278</v>
@@ -6430,11 +6444,14 @@
       <c r="O115" s="1">
         <v>27.39</v>
       </c>
-      <c r="P115" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P115" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q115" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A116" s="1" t="s">
         <v>113</v>
       </c>
@@ -6454,7 +6471,7 @@
         <v>230</v>
       </c>
       <c r="M116" s="1" t="s">
-        <v>377</v>
+        <v>334</v>
       </c>
       <c r="N116" s="1" t="s">
         <v>277</v>
@@ -6462,11 +6479,14 @@
       <c r="O116" s="1">
         <v>1</v>
       </c>
-      <c r="P116" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P116" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q116" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A117" s="1" t="s">
         <v>113</v>
       </c>
@@ -6489,7 +6509,7 @@
         <v>236</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>378</v>
+        <v>335</v>
       </c>
       <c r="N117" s="1" t="s">
         <v>277</v>
@@ -6497,11 +6517,11 @@
       <c r="O117" s="1">
         <v>13</v>
       </c>
-      <c r="P117" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P117" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A118" s="1" t="s">
         <v>113</v>
       </c>
@@ -6521,7 +6541,7 @@
         <v>236</v>
       </c>
       <c r="M118" s="1" t="s">
-        <v>378</v>
+        <v>335</v>
       </c>
       <c r="N118" s="1" t="s">
         <v>277</v>
@@ -6529,11 +6549,11 @@
       <c r="O118" s="1">
         <v>4</v>
       </c>
-      <c r="P118" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P118" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A119" s="1" t="s">
         <v>113</v>
       </c>
@@ -6561,11 +6581,11 @@
       <c r="O119" s="1">
         <v>133.41999999999999</v>
       </c>
-      <c r="P119" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P119" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
         <v>113</v>
       </c>
@@ -6590,11 +6610,11 @@
       <c r="O120" s="1">
         <v>41.05</v>
       </c>
-      <c r="P120" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P120" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A121" s="1" t="s">
         <v>241</v>
       </c>
@@ -6622,11 +6642,8 @@
       <c r="O121" s="1">
         <v>1.17</v>
       </c>
-      <c r="P121" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.5">
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A122" s="1" t="s">
         <v>241</v>
       </c>
@@ -6654,11 +6671,8 @@
       <c r="O122" s="1">
         <v>0.54</v>
       </c>
-      <c r="P122" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.5">
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A123" s="1" t="s">
         <v>241</v>
       </c>
@@ -6686,11 +6700,8 @@
       <c r="O123" s="1">
         <v>-0.06</v>
       </c>
-      <c r="P123" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.5">
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
         <v>241</v>
       </c>
@@ -6704,7 +6715,7 @@
         <v>268</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>379</v>
+        <v>336</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>274</v>
@@ -6718,11 +6729,8 @@
       <c r="O124" s="1">
         <v>0.59</v>
       </c>
-      <c r="P124" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.5">
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A125" s="1" t="s">
         <v>241</v>
       </c>
@@ -6742,7 +6750,7 @@
         <v>243</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>357</v>
+        <v>314</v>
       </c>
       <c r="N125" s="1" t="s">
         <v>244</v>
@@ -6751,10 +6759,10 @@
         <v>3</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.5">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A126" s="1" t="s">
         <v>241</v>
       </c>
@@ -6777,7 +6785,7 @@
         <v>248</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
       <c r="N126" s="1" t="s">
         <v>21</v>
@@ -6786,10 +6794,10 @@
         <v>0.43</v>
       </c>
       <c r="P126" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.5">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A127" s="1" t="s">
         <v>241</v>
       </c>
@@ -6809,7 +6817,7 @@
         <v>248</v>
       </c>
       <c r="M127" s="1" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
       <c r="N127" s="1" t="s">
         <v>21</v>
@@ -6818,10 +6826,10 @@
         <v>0.3</v>
       </c>
       <c r="P127" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.5">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A128" s="1" t="s">
         <v>241</v>
       </c>
@@ -6841,7 +6849,7 @@
         <v>248</v>
       </c>
       <c r="M128" s="1" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
       <c r="N128" s="1" t="s">
         <v>21</v>
@@ -6850,7 +6858,7 @@
         <v>0.2</v>
       </c>
       <c r="P128" s="1" t="s">
-        <v>311</v>
+        <v>382</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.5">
@@ -6876,7 +6884,7 @@
         <v>248</v>
       </c>
       <c r="M129" s="1" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
       <c r="N129" s="1" t="s">
         <v>21</v>
@@ -6885,7 +6893,7 @@
         <v>0.61</v>
       </c>
       <c r="P129" s="1" t="s">
-        <v>328</v>
+        <v>382</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.5">
@@ -6908,7 +6916,7 @@
         <v>248</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
       <c r="N130" s="1" t="s">
         <v>21</v>
@@ -6917,12 +6925,18 @@
         <v>0.38</v>
       </c>
       <c r="P130" s="1" t="s">
-        <v>352</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P48" r:id="rId1" display="https://www.huduser.gov/portal/NSP2datadesc.html" xr:uid="{D10C2A8B-6A08-459D-A691-DEEE1A4F8A18}"/>
+    <hyperlink ref="P49" r:id="rId2" display="https://www.huduser.gov/portal/NSP2datadesc.html" xr:uid="{B72060C0-609B-4BC3-BF1C-BB98E8F1923F}"/>
+    <hyperlink ref="Q48" r:id="rId3" display="https://www.consumerfinance.gov/data-research/mortgage-performance-trends/" xr:uid="{543867B2-6EC8-4982-B446-DE7366A07BCB}"/>
+    <hyperlink ref="Q49" r:id="rId4" display="https://www.consumerfinance.gov/data-research/mortgage-performance-trends/" xr:uid="{FC0E5034-573D-418C-9164-4E64FFAEB79A}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <ignoredErrors>
     <ignoredError sqref="O5:O6 O2:O3" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>